<commit_message>
ee sheet done with two items not matched edge case
</commit_message>
<xml_diff>
--- a/uploads/Blank BOQ AIS ASP Zeer รังสิต-1.xlsx
+++ b/uploads/Blank BOQ AIS ASP Zeer รังสิต-1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a677022/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ar677022/Desktop/backup/woodman/boq_app/uploads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D55A4437-F68C-4449-82D2-A041BCF8C780}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA9B3C86-4063-A148-86F5-469C41561AB1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20480" tabRatio="384" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20480" tabRatio="384" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sum Int.+ระบบ 13-05-68" sheetId="12" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="312">
   <si>
     <t>FOR :</t>
   </si>
@@ -1033,6 +1033,9 @@
   </si>
   <si>
     <t>สรุปใบเสนอราคา</t>
+  </si>
+  <si>
+    <t>รวมรายการที่ 3</t>
   </si>
 </sst>
 </file>
@@ -4628,6 +4631,15 @@
     <xf numFmtId="0" fontId="81" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="81" fillId="2" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="81" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="81" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="11" xfId="15" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4682,16 +4694,31 @@
     <xf numFmtId="0" fontId="81" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="71" fillId="2" borderId="1" xfId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="168" fontId="47" fillId="2" borderId="0" xfId="36" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="171" fontId="71" fillId="2" borderId="1" xfId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="73" fillId="2" borderId="49" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="71" fillId="2" borderId="1" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="73" fillId="2" borderId="95" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="71" fillId="2" borderId="1" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="73" fillId="2" borderId="96" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="2" borderId="61" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="2" borderId="62" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="2" borderId="63" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="73" fillId="2" borderId="48" xfId="244" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="46" fillId="2" borderId="48" xfId="244" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="167" fontId="79" fillId="2" borderId="0" xfId="36" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -4733,9 +4760,6 @@
     <xf numFmtId="164" fontId="41" fillId="2" borderId="87" xfId="58" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="73" fillId="2" borderId="48" xfId="244" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="41" fillId="2" borderId="99" xfId="58" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4745,28 +4769,16 @@
     <xf numFmtId="164" fontId="41" fillId="2" borderId="100" xfId="58" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="168" fontId="47" fillId="2" borderId="0" xfId="36" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="71" fillId="2" borderId="1" xfId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="73" fillId="2" borderId="49" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="171" fontId="71" fillId="2" borderId="1" xfId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="73" fillId="2" borderId="95" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="71" fillId="2" borderId="1" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="73" fillId="2" borderId="96" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="2" borderId="61" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="2" borderId="62" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="2" borderId="63" xfId="38" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="2" borderId="48" xfId="244" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="71" fillId="2" borderId="1" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="168" fontId="47" fillId="2" borderId="49" xfId="36" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -4810,15 +4822,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="81" fillId="2" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="81" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="81" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="247">
@@ -55468,14 +55471,14 @@
       <c r="D1" s="7"/>
     </row>
     <row r="2" spans="1:5" s="8" customFormat="1" ht="6.75" customHeight="1">
-      <c r="A2" s="417"/>
-      <c r="B2" s="417"/>
+      <c r="A2" s="420"/>
+      <c r="B2" s="420"/>
       <c r="C2" s="49"/>
       <c r="D2" s="49"/>
     </row>
     <row r="3" spans="1:5" s="8" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A3" s="417"/>
-      <c r="B3" s="417"/>
+      <c r="A3" s="420"/>
+      <c r="B3" s="420"/>
       <c r="C3" s="49"/>
       <c r="D3" s="49"/>
     </row>
@@ -55522,21 +55525,21 @@
       <c r="D9" s="19"/>
     </row>
     <row r="10" spans="1:5" ht="20" customHeight="1">
-      <c r="A10" s="410" t="s">
+      <c r="A10" s="413" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="412" t="s">
+      <c r="B10" s="415" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="413"/>
+      <c r="C10" s="416"/>
       <c r="D10" s="348" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="20" customHeight="1">
-      <c r="A11" s="411"/>
-      <c r="B11" s="414"/>
-      <c r="C11" s="415"/>
+      <c r="A11" s="414"/>
+      <c r="B11" s="417"/>
+      <c r="C11" s="418"/>
       <c r="D11" s="349" t="s">
         <v>12</v>
       </c>
@@ -55666,9 +55669,9 @@
     </row>
     <row r="23" spans="1:12" s="35" customFormat="1" ht="39" customHeight="1" thickTop="1">
       <c r="A23" s="33"/>
-      <c r="B23" s="416"/>
-      <c r="C23" s="416"/>
-      <c r="D23" s="416"/>
+      <c r="B23" s="419"/>
+      <c r="C23" s="419"/>
+      <c r="D23" s="419"/>
     </row>
     <row r="24" spans="1:12" s="35" customFormat="1" ht="24" customHeight="1">
       <c r="A24" s="36" t="s">
@@ -55718,7 +55721,7 @@
   </sheetPr>
   <dimension ref="A1:L98"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+    <sheetView zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
@@ -55741,15 +55744,15 @@
       <c r="E1" s="361"/>
     </row>
     <row r="2" spans="1:11" s="360" customFormat="1" ht="6.75" customHeight="1">
-      <c r="A2" s="421"/>
-      <c r="B2" s="421"/>
+      <c r="A2" s="424"/>
+      <c r="B2" s="424"/>
       <c r="C2" s="362"/>
       <c r="D2" s="362"/>
       <c r="E2" s="361"/>
     </row>
     <row r="3" spans="1:11" s="360" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A3" s="421"/>
-      <c r="B3" s="421"/>
+      <c r="A3" s="424"/>
+      <c r="B3" s="424"/>
       <c r="C3" s="362"/>
       <c r="D3" s="362"/>
       <c r="E3" s="361"/>
@@ -55800,36 +55803,36 @@
     </row>
     <row r="8" spans="1:11" ht="6.75" customHeight="1"/>
     <row r="9" spans="1:11" s="381" customFormat="1">
-      <c r="A9" s="422" t="s">
+      <c r="A9" s="425" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="424" t="s">
+      <c r="B9" s="427" t="s">
         <v>73</v>
       </c>
-      <c r="C9" s="426"/>
-      <c r="D9" s="424" t="s">
+      <c r="C9" s="429"/>
+      <c r="D9" s="427" t="s">
         <v>51</v>
       </c>
-      <c r="E9" s="424" t="s">
+      <c r="E9" s="427" t="s">
         <v>1</v>
       </c>
-      <c r="F9" s="418" t="s">
+      <c r="F9" s="421" t="s">
         <v>52</v>
       </c>
-      <c r="G9" s="419"/>
-      <c r="H9" s="420"/>
+      <c r="G9" s="422"/>
+      <c r="H9" s="423"/>
       <c r="I9" s="380" t="s">
         <v>3</v>
       </c>
-      <c r="J9" s="471"/>
-      <c r="K9" s="472"/>
+      <c r="J9" s="410"/>
+      <c r="K9" s="411"/>
     </row>
     <row r="10" spans="1:11" s="381" customFormat="1">
-      <c r="A10" s="423"/>
-      <c r="B10" s="425"/>
-      <c r="C10" s="427"/>
-      <c r="D10" s="425"/>
-      <c r="E10" s="425"/>
+      <c r="A10" s="426"/>
+      <c r="B10" s="428"/>
+      <c r="C10" s="430"/>
+      <c r="D10" s="428"/>
+      <c r="E10" s="428"/>
       <c r="F10" s="382" t="s">
         <v>53</v>
       </c>
@@ -55842,8 +55845,8 @@
       <c r="I10" s="409" t="s">
         <v>56</v>
       </c>
-      <c r="J10" s="472"/>
-      <c r="K10" s="472"/>
+      <c r="J10" s="411"/>
+      <c r="K10" s="411"/>
     </row>
     <row r="11" spans="1:11" s="142" customFormat="1" ht="18.75" customHeight="1">
       <c r="A11" s="138">
@@ -55859,8 +55862,8 @@
       <c r="G11" s="141"/>
       <c r="H11" s="141"/>
       <c r="I11" s="139"/>
-      <c r="J11" s="473"/>
-      <c r="K11" s="473"/>
+      <c r="J11" s="412"/>
+      <c r="K11" s="412"/>
     </row>
     <row r="12" spans="1:11" s="142" customFormat="1" ht="18.75" customHeight="1">
       <c r="A12" s="383">
@@ -57490,8 +57493,8 @@
   </sheetPr>
   <dimension ref="A1:M104"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="S26" sqref="S26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
@@ -57535,8 +57538,8 @@
       <c r="G2" s="53"/>
       <c r="H2" s="65"/>
       <c r="I2" s="65"/>
-      <c r="J2" s="432"/>
-      <c r="K2" s="432"/>
+      <c r="J2" s="440"/>
+      <c r="K2" s="440"/>
       <c r="L2" s="55"/>
     </row>
     <row r="3" spans="1:13" s="66" customFormat="1" ht="18.75" customHeight="1">
@@ -57553,8 +57556,8 @@
       <c r="G3" s="53"/>
       <c r="H3" s="54"/>
       <c r="I3" s="54"/>
-      <c r="J3" s="432"/>
-      <c r="K3" s="432"/>
+      <c r="J3" s="440"/>
+      <c r="K3" s="440"/>
       <c r="L3" s="55"/>
     </row>
     <row r="4" spans="1:13" s="71" customFormat="1" ht="18.75" customHeight="1">
@@ -57605,43 +57608,43 @@
       <c r="M6" s="101"/>
     </row>
     <row r="7" spans="1:13" s="76" customFormat="1" ht="20" customHeight="1">
-      <c r="A7" s="428" t="s">
+      <c r="A7" s="456" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="428" t="s">
+      <c r="B7" s="456" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="429" t="s">
+      <c r="C7" s="457" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="429"/>
-      <c r="E7" s="429"/>
-      <c r="F7" s="428" t="s">
+      <c r="D7" s="457"/>
+      <c r="E7" s="457"/>
+      <c r="F7" s="456" t="s">
         <v>1</v>
       </c>
-      <c r="G7" s="428" t="s">
+      <c r="G7" s="456" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="433" t="s">
+      <c r="H7" s="441" t="s">
         <v>25</v>
       </c>
-      <c r="I7" s="434"/>
-      <c r="J7" s="433" t="s">
+      <c r="I7" s="442"/>
+      <c r="J7" s="441" t="s">
         <v>26</v>
       </c>
-      <c r="K7" s="434"/>
+      <c r="K7" s="442"/>
       <c r="L7" s="75" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:13" s="76" customFormat="1" ht="20" customHeight="1">
-      <c r="A8" s="428"/>
-      <c r="B8" s="428"/>
-      <c r="C8" s="429"/>
-      <c r="D8" s="429"/>
-      <c r="E8" s="429"/>
-      <c r="F8" s="430"/>
-      <c r="G8" s="431"/>
+      <c r="A8" s="456"/>
+      <c r="B8" s="456"/>
+      <c r="C8" s="457"/>
+      <c r="D8" s="457"/>
+      <c r="E8" s="457"/>
+      <c r="F8" s="458"/>
+      <c r="G8" s="459"/>
       <c r="H8" s="77" t="s">
         <v>22</v>
       </c>
@@ -57851,11 +57854,11 @@
     <row r="17" spans="1:12" s="109" customFormat="1" ht="20.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="A17" s="284"/>
       <c r="B17" s="285"/>
-      <c r="C17" s="450" t="s">
+      <c r="C17" s="432" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="451"/>
-      <c r="E17" s="452"/>
+      <c r="D17" s="433"/>
+      <c r="E17" s="434"/>
       <c r="F17" s="286"/>
       <c r="G17" s="286"/>
       <c r="H17" s="287"/>
@@ -57869,11 +57872,11 @@
         <v>2</v>
       </c>
       <c r="B18" s="288"/>
-      <c r="C18" s="453" t="s">
+      <c r="C18" s="435" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="454"/>
-      <c r="E18" s="455"/>
+      <c r="D18" s="436"/>
+      <c r="E18" s="437"/>
       <c r="F18" s="289"/>
       <c r="G18" s="289"/>
       <c r="H18" s="117"/>
@@ -58005,11 +58008,11 @@
     <row r="24" spans="1:12" s="98" customFormat="1" ht="20.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="A24" s="284"/>
       <c r="B24" s="284"/>
-      <c r="C24" s="445" t="s">
+      <c r="C24" s="438" t="s">
         <v>38</v>
       </c>
-      <c r="D24" s="445"/>
-      <c r="E24" s="445"/>
+      <c r="D24" s="438"/>
+      <c r="E24" s="438"/>
       <c r="F24" s="286"/>
       <c r="G24" s="286"/>
       <c r="H24" s="110"/>
@@ -58111,9 +58114,11 @@
     <row r="29" spans="1:12" s="109" customFormat="1" ht="21" customHeight="1" thickTop="1" thickBot="1">
       <c r="A29" s="284"/>
       <c r="B29" s="284"/>
-      <c r="C29" s="445"/>
-      <c r="D29" s="445"/>
-      <c r="E29" s="445"/>
+      <c r="C29" s="438" t="s">
+        <v>311</v>
+      </c>
+      <c r="D29" s="438"/>
+      <c r="E29" s="438"/>
       <c r="F29" s="286"/>
       <c r="G29" s="286"/>
       <c r="H29" s="110"/>
@@ -58320,8 +58325,8 @@
       </c>
       <c r="H39" s="88"/>
       <c r="I39" s="79"/>
-      <c r="J39" s="441"/>
-      <c r="K39" s="442"/>
+      <c r="J39" s="449"/>
+      <c r="K39" s="450"/>
       <c r="L39" s="341"/>
     </row>
     <row r="40" spans="1:13" s="98" customFormat="1" ht="21" customHeight="1">
@@ -58344,8 +58349,8 @@
       </c>
       <c r="H40" s="88"/>
       <c r="I40" s="79"/>
-      <c r="J40" s="441"/>
-      <c r="K40" s="442"/>
+      <c r="J40" s="449"/>
+      <c r="K40" s="450"/>
       <c r="L40" s="341"/>
     </row>
     <row r="41" spans="1:13" s="98" customFormat="1" ht="21.75" customHeight="1">
@@ -58368,8 +58373,8 @@
       </c>
       <c r="H41" s="88"/>
       <c r="I41" s="79"/>
-      <c r="J41" s="441"/>
-      <c r="K41" s="442"/>
+      <c r="J41" s="449"/>
+      <c r="K41" s="450"/>
       <c r="L41" s="341"/>
     </row>
     <row r="42" spans="1:13" s="98" customFormat="1" ht="21" customHeight="1">
@@ -58392,8 +58397,8 @@
       </c>
       <c r="H42" s="88"/>
       <c r="I42" s="79"/>
-      <c r="J42" s="441"/>
-      <c r="K42" s="442"/>
+      <c r="J42" s="449"/>
+      <c r="K42" s="450"/>
       <c r="L42" s="341"/>
       <c r="M42" s="99"/>
     </row>
@@ -58415,11 +58420,11 @@
     <row r="44" spans="1:13" s="98" customFormat="1" ht="21.75" customHeight="1" thickTop="1" thickBot="1">
       <c r="A44" s="284"/>
       <c r="B44" s="284"/>
-      <c r="C44" s="445" t="s">
+      <c r="C44" s="438" t="s">
         <v>43</v>
       </c>
-      <c r="D44" s="445"/>
-      <c r="E44" s="445"/>
+      <c r="D44" s="438"/>
+      <c r="E44" s="438"/>
       <c r="F44" s="286"/>
       <c r="G44" s="286"/>
       <c r="H44" s="110"/>
@@ -58665,10 +58670,10 @@
       <c r="G55" s="82">
         <v>5</v>
       </c>
-      <c r="H55" s="441" t="s">
+      <c r="H55" s="449" t="s">
         <v>30</v>
       </c>
-      <c r="I55" s="442"/>
+      <c r="I55" s="450"/>
       <c r="J55" s="88"/>
       <c r="K55" s="80"/>
       <c r="L55" s="341"/>
@@ -58700,11 +58705,11 @@
     <row r="57" spans="1:12" ht="20" thickTop="1" thickBot="1">
       <c r="A57" s="284"/>
       <c r="B57" s="284"/>
-      <c r="C57" s="456" t="s">
+      <c r="C57" s="439" t="s">
         <v>47</v>
       </c>
-      <c r="D57" s="456"/>
-      <c r="E57" s="456"/>
+      <c r="D57" s="439"/>
+      <c r="E57" s="439"/>
       <c r="F57" s="286"/>
       <c r="G57" s="286"/>
       <c r="H57" s="110"/>
@@ -58750,10 +58755,10 @@
       <c r="G59" s="102">
         <v>1</v>
       </c>
-      <c r="H59" s="443" t="s">
+      <c r="H59" s="451" t="s">
         <v>214</v>
       </c>
-      <c r="I59" s="444"/>
+      <c r="I59" s="452"/>
       <c r="J59" s="80"/>
       <c r="K59" s="80"/>
       <c r="L59" s="341"/>
@@ -59025,11 +59030,11 @@
     <row r="71" spans="1:12" ht="20" thickTop="1" thickBot="1">
       <c r="A71" s="284"/>
       <c r="B71" s="284"/>
-      <c r="C71" s="445" t="s">
+      <c r="C71" s="438" t="s">
         <v>114</v>
       </c>
-      <c r="D71" s="445"/>
-      <c r="E71" s="445"/>
+      <c r="D71" s="438"/>
+      <c r="E71" s="438"/>
       <c r="F71" s="286"/>
       <c r="G71" s="286"/>
       <c r="H71" s="110"/>
@@ -59169,11 +59174,11 @@
     <row r="78" spans="1:12" ht="20" thickTop="1" thickBot="1">
       <c r="A78" s="284"/>
       <c r="B78" s="284"/>
-      <c r="C78" s="445" t="s">
+      <c r="C78" s="438" t="s">
         <v>228</v>
       </c>
-      <c r="D78" s="445"/>
-      <c r="E78" s="445"/>
+      <c r="D78" s="438"/>
+      <c r="E78" s="438"/>
       <c r="F78" s="286"/>
       <c r="G78" s="286"/>
       <c r="H78" s="110"/>
@@ -59323,11 +59328,11 @@
     <row r="85" spans="1:12" ht="20" thickTop="1" thickBot="1">
       <c r="A85" s="284"/>
       <c r="B85" s="284"/>
-      <c r="C85" s="445" t="s">
+      <c r="C85" s="438" t="s">
         <v>234</v>
       </c>
-      <c r="D85" s="445"/>
-      <c r="E85" s="445"/>
+      <c r="D85" s="438"/>
+      <c r="E85" s="438"/>
       <c r="F85" s="286"/>
       <c r="G85" s="286"/>
       <c r="H85" s="110"/>
@@ -59493,11 +59498,11 @@
     <row r="93" spans="1:12" ht="20" thickTop="1" thickBot="1">
       <c r="A93" s="284"/>
       <c r="B93" s="284"/>
-      <c r="C93" s="445" t="s">
+      <c r="C93" s="438" t="s">
         <v>239</v>
       </c>
-      <c r="D93" s="445"/>
-      <c r="E93" s="445"/>
+      <c r="D93" s="438"/>
+      <c r="E93" s="438"/>
       <c r="F93" s="286"/>
       <c r="G93" s="286"/>
       <c r="H93" s="110"/>
@@ -59542,13 +59547,13 @@
       <c r="G95" s="102">
         <v>6</v>
       </c>
-      <c r="H95" s="446" t="s">
+      <c r="H95" s="453" t="s">
         <v>214</v>
       </c>
-      <c r="I95" s="447"/>
-      <c r="J95" s="447"/>
-      <c r="K95" s="447"/>
-      <c r="L95" s="448"/>
+      <c r="I95" s="454"/>
+      <c r="J95" s="454"/>
+      <c r="K95" s="454"/>
+      <c r="L95" s="455"/>
     </row>
     <row r="96" spans="1:12" ht="18">
       <c r="A96" s="263"/>
@@ -59568,13 +59573,13 @@
       <c r="G96" s="102">
         <v>1</v>
       </c>
-      <c r="H96" s="446" t="s">
+      <c r="H96" s="453" t="s">
         <v>214</v>
       </c>
-      <c r="I96" s="447"/>
-      <c r="J96" s="447"/>
-      <c r="K96" s="447"/>
-      <c r="L96" s="448"/>
+      <c r="I96" s="454"/>
+      <c r="J96" s="454"/>
+      <c r="K96" s="454"/>
+      <c r="L96" s="455"/>
     </row>
     <row r="97" spans="1:12" ht="18">
       <c r="A97" s="263"/>
@@ -59594,13 +59599,13 @@
       <c r="G97" s="102">
         <v>1</v>
       </c>
-      <c r="H97" s="435" t="s">
+      <c r="H97" s="443" t="s">
         <v>214</v>
       </c>
-      <c r="I97" s="436"/>
-      <c r="J97" s="436"/>
-      <c r="K97" s="436"/>
-      <c r="L97" s="437"/>
+      <c r="I97" s="444"/>
+      <c r="J97" s="444"/>
+      <c r="K97" s="444"/>
+      <c r="L97" s="445"/>
     </row>
     <row r="98" spans="1:12" ht="18">
       <c r="A98" s="263"/>
@@ -59701,11 +59706,11 @@
     <row r="102" spans="1:12" ht="20" thickTop="1" thickBot="1">
       <c r="A102" s="284"/>
       <c r="B102" s="285"/>
-      <c r="C102" s="438" t="s">
+      <c r="C102" s="446" t="s">
         <v>247</v>
       </c>
-      <c r="D102" s="439"/>
-      <c r="E102" s="440"/>
+      <c r="D102" s="447"/>
+      <c r="E102" s="448"/>
       <c r="F102" s="284"/>
       <c r="G102" s="284"/>
       <c r="H102" s="320"/>
@@ -59717,9 +59722,9 @@
     <row r="103" spans="1:12" ht="25" thickTop="1" thickBot="1">
       <c r="A103" s="175"/>
       <c r="B103" s="175"/>
-      <c r="C103" s="449"/>
-      <c r="D103" s="449"/>
-      <c r="E103" s="449"/>
+      <c r="C103" s="431"/>
+      <c r="D103" s="431"/>
+      <c r="E103" s="431"/>
       <c r="F103" s="123"/>
       <c r="G103" s="123"/>
       <c r="H103" s="124"/>
@@ -59736,14 +59741,11 @@
     <row r="104" spans="1:12" ht="16" thickTop="1"/>
   </sheetData>
   <mergeCells count="29">
-    <mergeCell ref="C103:E103"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="C29:E29"/>
-    <mergeCell ref="C44:E44"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C71:E71"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="G7:G8"/>
     <mergeCell ref="J2:K3"/>
     <mergeCell ref="H7:I7"/>
     <mergeCell ref="J7:K7"/>
@@ -59760,11 +59762,14 @@
     <mergeCell ref="H96:L96"/>
     <mergeCell ref="C78:E78"/>
     <mergeCell ref="C85:E85"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="C103:E103"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="C29:E29"/>
+    <mergeCell ref="C44:E44"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C71:E71"/>
   </mergeCells>
   <pageMargins left="0.31496062992125984" right="0.15748031496062992" top="0.23622047244094491" bottom="0.19685039370078741" header="0.15748031496062992" footer="0.15748031496062992"/>
   <pageSetup paperSize="9" scale="60" orientation="portrait" r:id="rId1"/>
@@ -59868,43 +59873,43 @@
       <c r="L4" s="188"/>
     </row>
     <row r="5" spans="1:12" ht="21" thickTop="1">
-      <c r="A5" s="460" t="s">
+      <c r="A5" s="463" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="461" t="s">
+      <c r="B5" s="464" t="s">
         <v>73</v>
       </c>
-      <c r="C5" s="460" t="s">
+      <c r="C5" s="463" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="460"/>
-      <c r="E5" s="460"/>
-      <c r="F5" s="428" t="s">
+      <c r="D5" s="463"/>
+      <c r="E5" s="463"/>
+      <c r="F5" s="456" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="428" t="s">
+      <c r="G5" s="456" t="s">
         <v>21</v>
       </c>
-      <c r="H5" s="433" t="s">
+      <c r="H5" s="441" t="s">
         <v>25</v>
       </c>
-      <c r="I5" s="434"/>
-      <c r="J5" s="433" t="s">
+      <c r="I5" s="442"/>
+      <c r="J5" s="441" t="s">
         <v>26</v>
       </c>
-      <c r="K5" s="434"/>
+      <c r="K5" s="442"/>
       <c r="L5" s="75" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="23.25" customHeight="1">
-      <c r="A6" s="460"/>
-      <c r="B6" s="462"/>
-      <c r="C6" s="460"/>
-      <c r="D6" s="460"/>
-      <c r="E6" s="460"/>
-      <c r="F6" s="430"/>
-      <c r="G6" s="431"/>
+      <c r="A6" s="463"/>
+      <c r="B6" s="465"/>
+      <c r="C6" s="463"/>
+      <c r="D6" s="463"/>
+      <c r="E6" s="463"/>
+      <c r="F6" s="458"/>
+      <c r="G6" s="459"/>
       <c r="H6" s="77" t="s">
         <v>22</v>
       </c>
@@ -60383,11 +60388,11 @@
     <row r="28" spans="1:12" s="198" customFormat="1" ht="20.25" customHeight="1" thickTop="1" thickBot="1">
       <c r="A28" s="230"/>
       <c r="B28" s="231"/>
-      <c r="C28" s="457" t="s">
+      <c r="C28" s="460" t="s">
         <v>159</v>
       </c>
-      <c r="D28" s="458"/>
-      <c r="E28" s="459"/>
+      <c r="D28" s="461"/>
+      <c r="E28" s="462"/>
       <c r="F28" s="232"/>
       <c r="G28" s="232"/>
       <c r="H28" s="233"/>
@@ -60662,43 +60667,43 @@
       <c r="L6" s="246"/>
     </row>
     <row r="7" spans="1:12" ht="22.5" customHeight="1">
-      <c r="A7" s="460" t="s">
+      <c r="A7" s="463" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="467" t="s">
+      <c r="B7" s="470" t="s">
         <v>73</v>
       </c>
-      <c r="C7" s="460" t="s">
+      <c r="C7" s="463" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="460"/>
-      <c r="E7" s="460"/>
-      <c r="F7" s="468" t="s">
+      <c r="D7" s="463"/>
+      <c r="E7" s="463"/>
+      <c r="F7" s="471" t="s">
         <v>1</v>
       </c>
-      <c r="G7" s="468" t="s">
+      <c r="G7" s="471" t="s">
         <v>21</v>
       </c>
-      <c r="H7" s="465" t="s">
+      <c r="H7" s="468" t="s">
         <v>25</v>
       </c>
-      <c r="I7" s="466"/>
-      <c r="J7" s="465" t="s">
+      <c r="I7" s="469"/>
+      <c r="J7" s="468" t="s">
         <v>26</v>
       </c>
-      <c r="K7" s="466"/>
+      <c r="K7" s="469"/>
       <c r="L7" s="248" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:12">
-      <c r="A8" s="460"/>
-      <c r="B8" s="467"/>
-      <c r="C8" s="460"/>
-      <c r="D8" s="460"/>
-      <c r="E8" s="460"/>
-      <c r="F8" s="469"/>
-      <c r="G8" s="470"/>
+      <c r="A8" s="463"/>
+      <c r="B8" s="470"/>
+      <c r="C8" s="463"/>
+      <c r="D8" s="463"/>
+      <c r="E8" s="463"/>
+      <c r="F8" s="472"/>
+      <c r="G8" s="473"/>
       <c r="H8" s="249" t="s">
         <v>22</v>
       </c>
@@ -60741,10 +60746,10 @@
       <c r="C10" s="253" t="s">
         <v>24</v>
       </c>
-      <c r="D10" s="463" t="s">
+      <c r="D10" s="466" t="s">
         <v>162</v>
       </c>
-      <c r="E10" s="464"/>
+      <c r="E10" s="467"/>
       <c r="F10" s="254" t="s">
         <v>6</v>
       </c>
@@ -60807,11 +60812,11 @@
     <row r="14" spans="1:12" s="198" customFormat="1" ht="25" thickTop="1" thickBot="1">
       <c r="A14" s="230"/>
       <c r="B14" s="261"/>
-      <c r="C14" s="457" t="s">
+      <c r="C14" s="460" t="s">
         <v>159</v>
       </c>
-      <c r="D14" s="458"/>
-      <c r="E14" s="459"/>
+      <c r="D14" s="461"/>
+      <c r="E14" s="462"/>
       <c r="F14" s="232"/>
       <c r="G14" s="232"/>
       <c r="H14" s="233"/>

</xml_diff>